<commit_message>
Finish Problem Solving Quiz
</commit_message>
<xml_diff>
--- a/02 - Notes/01 - Problem Solving/Quiz/Scratch Work.xlsx
+++ b/02 - Notes/01 - Problem Solving/Quiz/Scratch Work.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://chickasawnation-my.sharepoint.com/personal/daniel_carpenter_chickasaw_net/Documents/Documents/GitHub/OU-DSA/Metaheuristics/02 - Notes/01 - Problem Solving/Quiz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCA7FDC8-A2F5-444F-8D93-9ECA5B9181B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{CCA7FDC8-A2F5-444F-8D93-9ECA5B9181B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{DE34C8D4-AD10-48D4-92F0-224934D63152}"/>
   <bookViews>
-    <workbookView xWindow="47715" yWindow="4620" windowWidth="15075" windowHeight="14805" xr2:uid="{91446298-1297-40A9-913F-D2F0979A3416}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{91446298-1297-40A9-913F-D2F0979A3416}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Michonne</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>sumProd</t>
+  </si>
+  <si>
+    <t>posilible routes</t>
   </si>
 </sst>
 </file>
@@ -619,7 +622,7 @@
   <dimension ref="A2:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,6 +644,9 @@
         <f>FACT(B2 - 1) / 2</f>
         <v>19958400</v>
       </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
@@ -821,79 +827,79 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D16" t="b">
-        <f>IF(NOT(D14), C14)</f>
+        <f t="shared" ref="D16:I16" si="2">IF(NOT(D14), C14)</f>
         <v>0</v>
       </c>
       <c r="E16" t="b">
-        <f>IF(NOT(E14), D14)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F16" t="b">
-        <f>IF(NOT(F14), E14)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G16" t="b">
-        <f>IF(NOT(G14), F14)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H16" t="b">
-        <f>IF(NOT(H14), G14)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I16" t="b">
-        <f>IF(NOT(I14), H14)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D18" t="b">
-        <f>IF(D14, NOT(C14))</f>
+        <f t="shared" ref="D18:I18" si="3">IF(D14, NOT(C14))</f>
         <v>0</v>
       </c>
       <c r="E18" t="b">
-        <f>IF(E14, NOT(D14))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F18" t="b">
-        <f>IF(F14, NOT(E14))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G18" t="b">
-        <f>IF(G14, NOT(F14))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H18" t="b">
-        <f>IF(H14, NOT(G14))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I18" t="b">
-        <f>IF(I14, NOT(H14))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D19" t="b">
-        <f>IF(NOT(D13), C13)</f>
+        <f t="shared" ref="D19:I19" si="4">IF(NOT(D13), C13)</f>
         <v>1</v>
       </c>
       <c r="E19" t="b">
-        <f>IF(NOT(E13), D13)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F19" t="b">
-        <f>IF(NOT(F13), E13)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G19" t="b">
-        <f>IF(NOT(G13), F13)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H19" t="b">
-        <f>IF(NOT(H13), G13)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I19" t="b">
-        <f>IF(NOT(I13), H13)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -903,23 +909,23 @@
         <v>0</v>
       </c>
       <c r="E21" t="b">
-        <f t="shared" ref="E21:I21" si="2">OR(AND(E15, E16), AND(E18, E19))</f>
+        <f t="shared" ref="E21:I21" si="5">OR(AND(E15, E16), AND(E18, E19))</f>
         <v>0</v>
       </c>
       <c r="F21" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G21" s="8" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H21" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I21" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>